<commit_message>
added kilp and fixed minor issue in date format fun
</commit_message>
<xml_diff>
--- a/GT/process_log.xlsx
+++ b/GT/process_log.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,7 +550,451 @@
           <t>Alcon_Document Expiration Report_05302022.xlsx</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>5/30/2022 15:44</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5/30/2022 15:52</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5/30/2022 16:26</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>5/30/2022 16:34</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>5/30/2022 16:40</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>5/30/2022 16:58</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>5/30/2022 17:04</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>5/30/2022 17:10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>5/30/2022 19:33</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5/30/2022 19:49</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>5/30/2022 19:55</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5/30/2022 20:02</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
corrected syntax error of quote
</commit_message>
<xml_diff>
--- a/GT/process_log.xlsx
+++ b/GT/process_log.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -994,7 +994,266 @@
           <t>Alcon_Document Expiration Report_05302022.xlsx</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>5/30/2022 21:51</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Monday</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05302022.xlsx</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05302022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5/31/2022 09:46</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Sent</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>5/31/2022 11:48</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Send Mail Disabled</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>5/31/2022 11:53</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Send Mail Disabled</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>5/31/2022 12:01</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Send Mail Disabled</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>5/31/2022 12:33</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Send Mail Disabled</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>5/31/2022 12:48</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Tuesday</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Alcon</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Processed</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Send Mail Disabled</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Alcon_Status Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Alcon_Document Expiration Report_05312022.xlsx</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>